<commit_message>
Integrate Results with Excel
Integrate Results with Excel
</commit_message>
<xml_diff>
--- a/POC/TestData/TestCasesData.xlsx
+++ b/POC/TestData/TestCasesData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>S.No</t>
   </si>
@@ -52,13 +52,22 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
+    <t>RunTime</t>
+  </si>
+  <si>
+    <t>11 Seconds</t>
+  </si>
+  <si>
+    <t>35 Seconds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,8 +97,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,10 +443,11 @@
     <col min="2" max="2" width="57" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,8 +469,11 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -472,8 +486,17 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="1">
+        <v>0.82754629629629628</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.82836805555555559</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -484,8 +507,485 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.82837962962962963</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.82878472222222221</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+    </row>
+    <row r="89" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+    </row>
+    <row r="90" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+    </row>
+    <row r="91" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+    </row>
+    <row r="92" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+    </row>
+    <row r="93" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+    </row>
+    <row r="96" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+    </row>
+    <row r="97" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+    </row>
+    <row r="99" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+    </row>
+    <row r="100" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+    </row>
+    <row r="101" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+    </row>
+    <row r="102" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+    </row>
+    <row r="103" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+    </row>
+    <row r="104" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+    </row>
+    <row r="105" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+    </row>
+    <row r="106" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+    </row>
+    <row r="107" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+    </row>
+    <row r="108" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+    </row>
+    <row r="109" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+    </row>
+    <row r="110" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+    </row>
+    <row r="111" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+    </row>
+    <row r="112" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+    </row>
+    <row r="113" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+    </row>
+    <row r="114" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+    </row>
+    <row r="115" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+    </row>
+    <row r="116" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+    </row>
+    <row r="117" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+    </row>
+    <row r="118" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+    </row>
+    <row r="119" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+    </row>
+    <row r="120" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>